<commit_message>
Costos Toma (Create, Update, Filter, Export)
</commit_message>
<xml_diff>
--- a/Service.Report/wwwroot/layout/excel/Indicators/CostoFijoListado.xlsx
+++ b/Service.Report/wwwroot/layout/excel/Indicators/CostoFijoListado.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.Report\wwwroot\layout\excel\Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB3194A5-2711-481B-93F1-FA7EE7511EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D122E8E4-03E7-47B9-A557-C716CD54E0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Promotions" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="CostosFijos" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Promotions">Promotions!$A$4:$E$5</definedName>
+    <definedName name="CostoToma">CostosFijos!$A$4:$C$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,13 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Clave</t>
-  </si>
-  <si>
-    <t>Activo</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <r>
       <rPr>
@@ -75,57 +68,12 @@
 DEL {{Fecha}} AL {{Fecha}}</t>
     </r>
   </si>
-  <si>
-    <t>Periodo</t>
-  </si>
-  <si>
-    <t>{{item.Clave}}</t>
-  </si>
-  <si>
-    <t>{{item.Nombre}}</t>
-  </si>
-  <si>
-    <t>{{item.Periodo}}</t>
-  </si>
-  <si>
-    <t>Lista</t>
-  </si>
-  <si>
-    <t>{{item.NombreListaPrecio}}</t>
-  </si>
-  <si>
-    <t>{{item.Activo}}</t>
-  </si>
-  <si>
-    <t>Nombre Promoción</t>
-  </si>
-  <si>
-    <t>Costo Mensual Fijo</t>
-  </si>
-  <si>
-    <t>{{Mes}}</t>
-  </si>
-  <si>
-    <t>{{item.Sucursal}}</t>
-  </si>
-  <si>
-    <t>{{item.Servicio}}</t>
-  </si>
-  <si>
-    <t>TOTAL MENSUAL</t>
-  </si>
-  <si>
-    <t>TOTAL DIARIO (24)</t>
-  </si>
-  <si>
-    <t>TOTAL SEMANAL (6)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,22 +120,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,32 +141,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -262,7 +199,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>773907</xdr:colOff>
+      <xdr:colOff>547688</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1466850</xdr:rowOff>
     </xdr:to>
@@ -605,14 +542,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:E5"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="4" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" customWidth="1"/>
@@ -620,52 +559,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>2</v>
+      <c r="A1" s="4" t="s">
+        <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
@@ -678,133 +595,4 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1477E2-9F08-4F36-B2FA-2D336C886EBF}">
-  <dimension ref="A1:P12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H4"/>
-  </mergeCells>
-  <conditionalFormatting sqref="C6">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(C6))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Costos fijos y costo toma metodos create, update y excel
</commit_message>
<xml_diff>
--- a/Service.Report/wwwroot/layout/excel/Indicators/CostoFijoListado.xlsx
+++ b/Service.Report/wwwroot/layout/excel/Indicators/CostoFijoListado.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JuanDanielGonzalezAl\Documents\Projects\API\Service.Report\wwwroot\layout\excel\Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D122E8E4-03E7-47B9-A557-C716CD54E0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52CC18A-CD53-4491-B09E-A8D54F8FAA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="CostosFijos" sheetId="1" r:id="rId1"/>
+    <sheet name="CostoFijo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="CostoToma">CostosFijos!$A$4:$C$5</definedName>
+    <definedName name="CostoToma">CostoFijo!$A$4:$C$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -143,39 +143,18 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -540,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,34 +538,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="117" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+    <row r="3" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+    <row r="4" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="5"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D12" s="2"/>
-    </row>
+    <row r="13" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="40" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="41" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="42" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="44" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="45" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="46" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="47" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="48" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="49" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="50" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="53" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>

</xml_diff>